<commit_message>
Added crude total effects to table 3
</commit_message>
<xml_diff>
--- a/table3.xlsx
+++ b/table3.xlsx
@@ -10,14 +10,14 @@
     <sheet name="table3" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="table3">'table3'!$A$1:$J$10</definedName>
+    <definedName name="table3">'table3'!$A$1:$M$9</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>param</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>pir_cat 200%+</t>
+  </si>
+  <si>
+    <t>est_TE_crude</t>
+  </si>
+  <si>
+    <t>lwr_TE_crude</t>
+  </si>
+  <si>
+    <t>upr_TE_crude</t>
   </si>
 </sst>
 </file>
@@ -142,9 +151,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AAA1048576"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -160,9 +169,12 @@
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -193,194 +205,270 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>2.42913387287519e-001</v>
+        <v>.24291338728750958</v>
       </c>
       <c r="C2">
-        <v>1.5770717938613964e-001</v>
+        <v>.15770717938613038</v>
       </c>
       <c r="D2">
-        <v>3.2811959518889844e-001</v>
+        <v>.3281195951888888</v>
       </c>
       <c r="E2">
-        <v>-1.3161717236386838e-002</v>
+        <v>-.013161717236386844</v>
       </c>
       <c r="F2">
-        <v>-2.3587414171106076e-002</v>
+        <v>-.02358741417110608</v>
       </c>
       <c r="G2">
-        <v>-4.0737626212627176e-003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-.0040737626212627165</v>
+      </c>
+      <c r="K2">
+        <v>.16341024123474343</v>
+      </c>
+      <c r="L2">
+        <v>.07140327928625073</v>
+      </c>
+      <c r="M2">
+        <v>.25541720318323613</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.e+000</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.e+000</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.e+000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>-.2784872528661817</v>
+      </c>
+      <c r="L3">
+        <v>-.3571219289851188</v>
+      </c>
+      <c r="M3">
+        <v>-.1998525767472446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>2.1485099728507152e-001</v>
+        <v>.21485099728507454</v>
       </c>
       <c r="C4">
-        <v>1.4923754362512218e-001</v>
+        <v>.14923754362512548</v>
       </c>
       <c r="D4">
-        <v>2.8046445094502072e-001</v>
+        <v>.2804644509450236</v>
       </c>
       <c r="E4">
-        <v>-1.0375900252843184e-002</v>
+        <v>-.01037590025284318</v>
       </c>
       <c r="F4">
-        <v>-1.8479323706812272e-002</v>
+        <v>-.018479323706812274</v>
       </c>
       <c r="G4">
-        <v>-3.1617106708323096e-003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-.0031617106708323097</v>
+      </c>
+      <c r="K4">
+        <v>.10262579001871396</v>
+      </c>
+      <c r="L4">
+        <v>.027223279317197827</v>
+      </c>
+      <c r="M4">
+        <v>.17802830072023007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1.8469761295441796e-001</v>
+        <v>.18469761295440953</v>
       </c>
       <c r="C5">
-        <v>9.7842417466335936e-002</v>
+        <v>.09784241746632819</v>
       </c>
       <c r="D5">
-        <v>2.7155280844249996e-001</v>
+        <v>.27155280844249086</v>
       </c>
       <c r="E5">
-        <v>-1.2393713629959164e-002</v>
+        <v>-.012393713629959164</v>
       </c>
       <c r="F5">
-        <v>-2.292267750347092e-002</v>
+        <v>-.02292267750347092</v>
       </c>
       <c r="G5">
-        <v>-3.8792552784562528e-003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-.0038792552784562527</v>
+      </c>
+      <c r="K5">
+        <v>.15296185129777679</v>
+      </c>
+      <c r="L5">
+        <v>.06721573324221719</v>
+      </c>
+      <c r="M5">
+        <v>.23870796935333638</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6">
-        <v>1.3438256788187804e-001</v>
+        <v>.1343825678818791</v>
       </c>
       <c r="C6">
-        <v>6.3776917012284176e-002</v>
+        <v>.0637769170122852</v>
       </c>
       <c r="D6">
-        <v>2.0498821875147204e-001</v>
+        <v>.204988218751473</v>
       </c>
       <c r="E6">
-        <v>-9.4552920504418976e-003</v>
+        <v>-.009455292050441896</v>
       </c>
       <c r="F6">
-        <v>-1.719448099578656e-002</v>
+        <v>-.017194480995786562</v>
       </c>
       <c r="G6">
-        <v>-2.9859688474248556e-003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-.0029859688474248563</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>1.559140934508089e-001</v>
+        <v>.1559140934508193</v>
       </c>
       <c r="C7">
-        <v>9.3727798679149248e-002</v>
+        <v>.09372779867915967</v>
       </c>
       <c r="D7">
-        <v>2.1810038822246856e-001</v>
+        <v>.21810038822247893</v>
       </c>
       <c r="E7">
-        <v>-1.0234591810922182e-002</v>
+        <v>-.010234591810922185</v>
       </c>
       <c r="F7">
-        <v>-1.8223886314437264e-002</v>
+        <v>-.018223886314437263</v>
       </c>
       <c r="G7">
-        <v>-3.420613791139378e-003</v>
+        <v>-.0034206137911393774</v>
       </c>
       <c r="H7">
-        <v>7.04934004324508e-003</v>
+        <v>.0070493400432450806</v>
       </c>
       <c r="I7">
-        <v>6.722708653019608e-004</v>
+        <v>.0006722708653019608</v>
       </c>
       <c r="J7">
-        <v>1.6626867509228196e-002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>.01662686750922819</v>
+      </c>
+      <c r="K7">
+        <v>.19259133970069062</v>
+      </c>
+      <c r="L7">
+        <v>.12818017243837104</v>
+      </c>
+      <c r="M7">
+        <v>.2570025069630102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>.10694518928460824</v>
+      </c>
+      <c r="C8">
+        <v>.05130032798409047</v>
+      </c>
+      <c r="D8">
+        <v>.162590050585126</v>
+      </c>
+      <c r="E8">
+        <v>-.007744371087658888</v>
+      </c>
+      <c r="F8">
+        <v>-.014648223733092363</v>
+      </c>
+      <c r="G8">
+        <v>-.0027594369307493483</v>
       </c>
       <c r="H8">
-        <v>1.1272725188090876e-003</v>
+        <v>.0011272725188090874</v>
       </c>
       <c r="I8">
-        <v>-2.417698287119408e-003</v>
+        <v>-.0024176982871194084</v>
       </c>
       <c r="J8">
-        <v>5.7235205632479584e-003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>.005723520563247956</v>
+      </c>
+      <c r="K8">
+        <v>.19119702316494017</v>
+      </c>
+      <c r="L8">
+        <v>.11622020610752454</v>
+      </c>
+      <c r="M8">
+        <v>.2661738402223558</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>1.0694518928460076e-001</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>5.1300327984082408e-002</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1.625900505851191e-001</v>
-      </c>
-      <c r="E9">
-        <v>-7.744371087658888e-003</v>
-      </c>
-      <c r="F9">
-        <v>-1.4648223733092362e-002</v>
-      </c>
-      <c r="G9">
-        <v>-2.7594369307493496e-003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10">
-        <v>0.e+000</v>
-      </c>
-      <c r="C10">
-        <v>0.e+000</v>
-      </c>
-      <c r="D10">
-        <v>0.e+000</v>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>